<commit_message>
update mappings for graduationDate
</commit_message>
<xml_diff>
--- a/data_dictionary/Jupiter OAI mapping.xlsx
+++ b/data_dictionary/Jupiter OAI mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="OAI mappings" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="196">
   <si>
     <t xml:space="preserve">HyrdraNorth to Jupiter OAI Mapping</t>
   </si>
@@ -54,25 +54,7 @@
     <t xml:space="preserve">In jupiter, all non-thesis items receive dc:type (bibo:report, bibo:article, etc.). Theses, however, receive their own RDF class (bibo:thesis), and do not have a dc:type.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">rdf:type with value </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">http://purl.org/ontology/bibo/Thesis</t>
-    </r>
+    <t xml:space="preserve">rdf:type with value http://purl.org/ontology/bibo/Thesis</t>
   </si>
   <si>
     <t xml:space="preserve">etd_ms:type</t>
@@ -193,6 +175,9 @@
   </si>
   <si>
     <t xml:space="preserve">http://purl.org/dc/terms/dateAccepted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://terms.library.ualberta.ca/date/graduationdate</t>
   </si>
   <si>
     <t xml:space="preserve">dc:date (theses only)</t>
@@ -758,35 +743,34 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.4336734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.2091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.1989795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="71.5459183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="43.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="71.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -834,7 +818,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1044,164 +1028,164 @@
         <v>50</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>8</v>
@@ -1209,13 +1193,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="0" t="s">
         <v>83</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>82</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>8</v>
@@ -1223,13 +1207,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>8</v>
@@ -1237,30 +1221,30 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1271,11 +1255,11 @@
     <mergeCell ref="C10:C11"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="http://purl.org/ontology/bibo/Thesis"/>
+    <hyperlink ref="B4" r:id="rId1" display="rdf:type with value http://purl.org/ontology/bibo/Thesis"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1284,132 +1268,131 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.85"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1418,7 +1401,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1427,67 +1410,66 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="71.8163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="71.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B8" s="7"/>
     </row>
@@ -1496,463 +1478,463 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B12" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>